<commit_message>
Data consolidation, renamed some stats to avoid 2 letter conflicts
</commit_message>
<xml_diff>
--- a/Proto/core/assets/ur data/data.xlsx
+++ b/Proto/core/assets/ur data/data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="185">
   <si>
     <t xml:space="preserve">internal_name</t>
   </si>
@@ -397,10 +397,10 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Attack Power</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AP</t>
+    <t xml:space="preserve">Impact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IM</t>
   </si>
   <si>
     <t xml:space="preserve">Max</t>
@@ -599,6 +599,9 @@
     <t xml:space="preserve">Appearance</t>
   </si>
   <si>
+    <t xml:space="preserve">AP</t>
+  </si>
+  <si>
     <t xml:space="preserve">Conviction</t>
   </si>
   <si>
@@ -611,43 +614,52 @@
     <t xml:space="preserve">AU</t>
   </si>
   <si>
-    <t xml:space="preserve">Vision</t>
+    <t xml:space="preserve">Sight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hearing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Structure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Life Force</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vitality</t>
   </si>
   <si>
     <t xml:space="preserve">VI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hearing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Opacity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Life Force</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitality</t>
   </si>
   <si>
     <t xml:space="preserve">Spirit</t>
@@ -699,7 +711,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -742,13 +754,6 @@
       <vertAlign val="subscript"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF800000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -796,7 +801,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -818,10 +823,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -850,16 +851,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="5.66836734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="5.66836734693878"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="5.53571428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="5.53571428571429"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="5.66836734693878"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="5.53571428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -915,21 +916,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="5.66836734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="5.66836734693878"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="5.53571428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="5.53571428571429"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="5.66836734693878"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="5.53571428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="1" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1000,17 +1001,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="5.66836734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="5.53571428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.58673469387755"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="5.66836734693878"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="5.53571428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="1" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1092,23 +1093,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="5.66836734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="5.53571428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.1224489795918"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="5.66836734693878"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="28.3469387755102"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="5.53571428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="27.9438775510204"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="1" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1415,30 +1416,30 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="5.66836734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="5.66836734693878"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="5.53571428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="5.53571428571429"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="5.66836734693878"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="27.1326530612245"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="23.219387755102"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="28.7551020408163"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="5.53571428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="26.7295918367347"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="28.3469387755102"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="1" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1542,36 +1543,36 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="5.66836734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="5.53571428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.8010204081633"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="5.66836734693878"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="11" min="9" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="17" min="16" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="11.4744897959184"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="23" min="22" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="14.4438775510204"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="3.78061224489796"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="1" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="34" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="5.53571428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="9" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="17" min="16" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="23" min="22" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="3.64285714285714"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="34" style="1" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1819,16 +1820,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="5.66836734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="5.66836734693878"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="5.53571428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="5.53571428571429"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="5.66836734693878"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="5.53571428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1876,25 +1877,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.6683673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.6989795918367"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.265306122449"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="32.8010204081633"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="65.0663265306122"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.4744897959184"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="32.3979591836735"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="64.2551020408163"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="11.0714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2064,136 +2065,144 @@
       <c r="A14" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>117</v>
+      <c r="B14" s="5" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>155</v>
+        <v>167</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
putting together data by hand in code to test out the structures
</commit_message>
<xml_diff>
--- a/Proto/core/assets/ur data/data.xlsx
+++ b/Proto/core/assets/ur data/data.xlsx
@@ -5,20 +5,21 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="EpiData Common" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Element" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Biome" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Humanoid" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Condition Blueprint" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Creature Blueprint" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Physical Blueprint" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="Stat Sets" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="Stats" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="enums" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="Body Part (DEP)" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="Creature Blueprint" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Physical Blueprint" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Condition Blueprint" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Modification" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Stat Sets" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Stats" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="enums" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="Body Part (DEP)" sheetId="12" state="visible" r:id="rId13"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="289">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -275,6 +276,168 @@
     <t xml:space="preserve">shirt, pants, hat, shoe, shoe</t>
   </si>
   <si>
+    <t xml:space="preserve">symbol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">body</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aliases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modifications</t>
+  </si>
+  <si>
+    <t xml:space="preserve">becomes_on_element</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skills</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abilities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conditions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inventory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">animal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">base animal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">all-corpse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Small rodent that normally eats roots and bark.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quadruped</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mouse, hampster, gerbil, shrew</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A regular person.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">humanoid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">possible aliases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">possible modifications</t>
+  </si>
+  <si>
+    <t xml:space="preserve">when used as material</t>
+  </si>
+  <si>
+    <t xml:space="preserve">passthrough resistances</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elemental damage multiplyer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">light emitted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">light emitted strength</t>
+  </si>
+  <si>
+    <t xml:space="preserve">possible conditions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">initial stats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">common inventory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">physical drops</t>
+  </si>
+  <si>
+    <t xml:space="preserve">element drops</t>
+  </si>
+  <si>
+    <t xml:space="preserve">identification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rarity modifications</t>
+  </si>
+  <si>
+    <t xml:space="preserve">base value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">creature data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">possible professions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ammunition data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">container data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grouping data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interactable data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">liquid data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">legible data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wearable data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wieldable data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zappable data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Animals are alive and can do things.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Base for all animals.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">brown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average human person.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">atomic tangerine</t>
+  </si>
+  <si>
     <t xml:space="preserve">duration</t>
   </si>
   <si>
@@ -305,166 +468,46 @@
     <t xml:space="preserve">suppresses</t>
   </si>
   <si>
-    <t xml:space="preserve">symbol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">body</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aliases</t>
-  </si>
-  <si>
-    <t xml:space="preserve">modifications</t>
-  </si>
-  <si>
-    <t xml:space="preserve">becomes_on_element</t>
-  </si>
-  <si>
-    <t xml:space="preserve">skills</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abilities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">conditions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inventory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">animal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">base animal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">all-corpse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vole</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Small rodent that normally eats roots and bark.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">v</t>
-  </si>
-  <si>
-    <t xml:space="preserve">quadruped</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mouse, hampster, gerbil, shrew</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A regular person.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">humanoid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">possible aliases</t>
-  </si>
-  <si>
-    <t xml:space="preserve">possible modifications</t>
-  </si>
-  <si>
-    <t xml:space="preserve">when used as material</t>
-  </si>
-  <si>
-    <t xml:space="preserve">passthrough resistances</t>
-  </si>
-  <si>
-    <t xml:space="preserve">elemental damage multiplyer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">light emitted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">light emitted strength</t>
-  </si>
-  <si>
-    <t xml:space="preserve">possible conditions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">initial stats</t>
-  </si>
-  <si>
-    <t xml:space="preserve">common inventory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">physical drops</t>
-  </si>
-  <si>
-    <t xml:space="preserve">element drops</t>
-  </si>
-  <si>
-    <t xml:space="preserve">identification</t>
-  </si>
-  <si>
-    <t xml:space="preserve">generic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rarity modifications</t>
-  </si>
-  <si>
-    <t xml:space="preserve">base value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">creature data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">possible professions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ammunition data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">container data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grouping data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">interactable data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">liquid data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">legible data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wearable data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wieldable data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zappable data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Animals are alive and can do things.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Base for all animals.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">brown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average human person.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">atomic tangerine</t>
+    <t xml:space="preserve">very tired</t>
+  </si>
+  <si>
+    <t xml:space="preserve">need rest badly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">this is when Rest gets very low</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parent overwrite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">counts as overwrite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">counts as gained</t>
+  </si>
+  <si>
+    <t xml:space="preserve">counts as lost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">possible prefix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">possible postfix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">color overwrite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">color multiply</t>
+  </si>
+  <si>
+    <t xml:space="preserve">light emitted strength changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">light emitted overwrite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">light emitted multiply</t>
   </si>
   <si>
     <t xml:space="preserve">Aim</t>
@@ -1278,15 +1321,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1424,43 +1467,340 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ6"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="19.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="25.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="31.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="63.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="11.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="10.8"/>
+  </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="AMJ1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>196</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>159</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>160</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>57</v>
+        <v>161</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>162</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>60</v>
+        <v>163</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="G8" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -1475,6 +1815,64 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AMJ6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="13.06"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1496,7 +1894,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="5.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="10.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="27.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="27.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="13.23"/>
@@ -1508,19 +1906,19 @@
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>234</v>
+        <v>248</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>235</v>
+        <v>249</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>236</v>
+        <v>250</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>237</v>
+        <v>251</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>1</v>
@@ -1529,87 +1927,87 @@
         <v>2</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>238</v>
+        <v>252</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>239</v>
+        <v>253</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>240</v>
+        <v>254</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>242</v>
+        <v>256</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>243</v>
+        <v>257</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>244</v>
+        <v>258</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="2" s="6" customFormat="true" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="B2" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="L2" s="6" t="n">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="2" s="5" customFormat="true" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="B2" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="L2" s="5" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="M2" s="6" t="n">
+      <c r="M2" s="5" t="n">
         <v>100</v>
       </c>
-      <c r="N2" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="P2" s="6" t="n">
+      <c r="N2" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" s="5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>251</v>
+        <v>265</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>247</v>
+        <v>261</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>252</v>
+        <v>266</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>253</v>
+        <v>267</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>254</v>
+        <v>268</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>255</v>
+        <v>269</v>
       </c>
       <c r="L3" s="1" t="n">
         <f aca="false">TRUE()</f>
@@ -1630,22 +2028,22 @@
     </row>
     <row r="4" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>255</v>
+        <v>269</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>256</v>
+        <v>270</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>257</v>
+        <v>271</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>258</v>
+        <v>272</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>259</v>
+        <v>273</v>
       </c>
       <c r="L4" s="1" t="n">
         <f aca="false">TRUE()</f>
@@ -1666,22 +2064,22 @@
     </row>
     <row r="5" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>260</v>
+        <v>274</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>247</v>
+        <v>261</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>262</v>
+        <v>276</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>263</v>
+        <v>277</v>
       </c>
       <c r="L5" s="1" t="n">
         <f aca="false">TRUE()</f>
@@ -1699,25 +2097,25 @@
     </row>
     <row r="6" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>263</v>
+        <v>277</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>247</v>
+        <v>261</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>264</v>
+        <v>278</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>265</v>
+        <v>279</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>266</v>
+        <v>280</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>267</v>
+        <v>281</v>
       </c>
       <c r="N6" s="1" t="n">
         <v>3</v>
@@ -1731,19 +2129,19 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>268</v>
+        <v>282</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>247</v>
+        <v>261</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>269</v>
+        <v>283</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>270</v>
+        <v>284</v>
       </c>
       <c r="M7" s="1" t="n">
         <v>20</v>
@@ -1760,30 +2158,30 @@
     </row>
     <row r="8" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>271</v>
+        <v>285</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>268</v>
+        <v>282</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>272</v>
+        <v>286</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>273</v>
+        <v>287</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>268</v>
+        <v>282</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>274</v>
+        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -1810,8 +2208,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1852,7 +2252,7 @@
       <c r="C3" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1866,7 +2266,7 @@
       <c r="C4" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1880,7 +2280,7 @@
       <c r="C5" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1896,7 +2296,7 @@
       <c r="A7" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1904,7 +2304,7 @@
       <c r="A8" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1915,7 +2315,7 @@
       <c r="B9" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F9" s="0" t="s">
@@ -1929,7 +2329,7 @@
       <c r="B10" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="4" t="s">
         <v>21</v>
       </c>
       <c r="F10" s="0" t="s">
@@ -1940,7 +2340,7 @@
       <c r="A11" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1948,7 +2348,7 @@
       <c r="A12" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1956,7 +2356,7 @@
       <c r="A13" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1964,7 +2364,7 @@
       <c r="A14" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1972,7 +2372,7 @@
       <c r="A15" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1980,7 +2380,7 @@
       <c r="A16" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1991,10 +2391,10 @@
       <c r="C17" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="E17" s="4" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2007,7 +2407,7 @@
       <c r="A19" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" s="4" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2015,7 +2415,7 @@
       <c r="A20" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" s="4" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2023,7 +2423,7 @@
       <c r="A21" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" s="4" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2036,7 +2436,7 @@
       <c r="A23" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D23" s="4" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2044,7 +2444,7 @@
       <c r="A24" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" s="4" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2052,7 +2452,7 @@
       <c r="A25" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="D25" s="4" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2060,7 +2460,7 @@
       <c r="A26" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="D26" s="4" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2068,7 +2468,7 @@
       <c r="A27" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="0" t="s">
+      <c r="D27" s="4" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2076,7 +2476,7 @@
       <c r="A28" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="D28" s="0" t="s">
+      <c r="D28" s="4" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2183,10 +2583,10 @@
       <c r="B2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="5" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2197,10 +2597,10 @@
       <c r="B3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="5" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2211,10 +2611,10 @@
       <c r="B4" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="5" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2225,10 +2625,10 @@
       <c r="B5" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="5" t="s">
         <v>57</v>
       </c>
       <c r="G5" s="1" t="s">
@@ -2242,10 +2642,10 @@
       <c r="B6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="5" t="s">
         <v>57</v>
       </c>
       <c r="G6" s="1" t="s">
@@ -2259,10 +2659,10 @@
       <c r="B7" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="5" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2273,10 +2673,10 @@
       <c r="B8" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="5" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2293,10 +2693,10 @@
       <c r="D9" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="5" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2324,17 +2724,17 @@
   </sheetPr>
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="30.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="30.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="40.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="57.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="57.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1013" min="6" style="1" width="8.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1014" style="0" width="8.37"/>
   </cols>
@@ -2397,80 +2797,6 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="1" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.47"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="1" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" s="2" customFormat="true" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:AMJ4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -2480,7 +2806,7 @@
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="29.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="29.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="10.53"/>
@@ -2508,31 +2834,31 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="ALQ1" s="0"/>
       <c r="ALR1" s="0"/>
@@ -2557,39 +2883,39 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2597,16 +2923,229 @@
         <v>77</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AL3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S3" activeCellId="0" sqref="S3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="18.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="12.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="15.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="14.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="13.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="12.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="10.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="17.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="21" style="1" width="8.37"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="2" customFormat="true" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="Q1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="W2" s="6" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="Z2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>111</v>
+      <c r="G3" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -2625,38 +3164,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AL3"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S3" activeCellId="0" sqref="S3"/>
+      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="18.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="10.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="12.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="15.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="14.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="8.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="13.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="12.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="12.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="10.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="17.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="21" style="1" width="8.37"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.47"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="1" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="2" customFormat="true" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2670,155 +3192,54 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>4</v>
+        <v>135</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>91</v>
+        <v>136</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>5</v>
+        <v>137</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>112</v>
+        <v>138</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>113</v>
+        <v>139</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>94</v>
+        <v>140</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>114</v>
+        <v>141</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>115</v>
+        <v>142</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>116</v>
+        <v>143</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="AH1" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="AK1" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="AL1" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>100</v>
+        <v>145</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="W2" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>77</v>
+        <v>147</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -2837,6 +3258,90 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:P1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="1" style="0" width="19.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="7.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="19.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="27.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="21.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="20.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="17" style="0" width="19.86"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AH6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -2845,8 +3350,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2860,105 +3367,105 @@
         <v>3</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>145</v>
+        <v>159</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>146</v>
+        <v>160</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>149</v>
+        <v>163</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>150</v>
+        <v>164</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>153</v>
+        <v>167</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>155</v>
+        <v>169</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>160</v>
+        <v>174</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>163</v>
+        <v>177</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>164</v>
+        <v>178</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
       <c r="Y1" s="3" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="Z1" s="3" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="AA1" s="3" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
       <c r="AB1" s="3" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="AC1" s="3" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="AD1" s="3" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="AE1" s="3" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="AF1" s="3" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="AG1" s="3" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="AH1" s="3" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>177</v>
+        <v>191</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>0</v>
@@ -3056,10 +3563,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>178</v>
+        <v>192</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>1</v>
@@ -3160,10 +3667,10 @@
         <v>77</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>179</v>
+        <v>193</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>50</v>
@@ -3261,13 +3768,13 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>180</v>
+        <v>194</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>181</v>
+        <v>195</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>80</v>
@@ -3355,356 +3862,4 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:J32"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="19.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="25.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="31.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="63.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="11.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="10.8"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>195</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>199</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>204</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="C8" s="5"/>
-      <c r="G8" s="0" t="s">
-        <v>208</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>171</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>172</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="B30" s="0" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>232</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>